<commit_message>
Avances al 3 de Abril
Se avanzaron las correcciones de ccc, falta terminar discusión con
temas de tabs abiertos en Chrome y falta Resumen
</commit_message>
<xml_diff>
--- a/requerimientos.xlsx
+++ b/requerimientos.xlsx
@@ -752,15 +752,16 @@
   <dimension ref="B2:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="32" x14ac:dyDescent="0.2">

</xml_diff>